<commit_message>
cập nhật mẫu file excel cho a Kiên
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/ThongDiep/BangKeSaiSot_TheoHoaDon.xlsx
+++ b/API/wwwroot/docs/ThongDiep/BangKeSaiSot_TheoHoaDon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NGO_VAN_CANH\PROJECTS\HOA_DON_DIEN_TU_BANMOI\Back-End\API\wwwroot\docs\ThongDiep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\hoadon-da.pmbk.vn\wwwroot\docs\ThongDiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -171,8 +171,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -180,14 +180,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,28 +472,28 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="24.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="31.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="18" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="31.7109375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" style="5" customWidth="1"/>
+    <col min="16" max="16" width="27.7109375" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -587,7 +587,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K5" s="5"/>
+      <c r="K5" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
fix lấy số lượng thông báo sai sót chưa lập thông báo và file excel bảng kê sai sót
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/ThongDiep/BangKeSaiSot_TheoHoaDon.xlsx
+++ b/API/wwwroot/docs/ThongDiep/BangKeSaiSot_TheoHoaDon.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\bill-back-end\API\wwwroot\docs\ThongDiep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanlt\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +143,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -149,7 +167,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,34 +205,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -495,86 +527,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.6640625" style="3" customWidth="1"/>
-    <col min="3" max="4" width="20.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="21.88671875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="18" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="23.21875" style="3" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" style="3" customWidth="1"/>
     <col min="11" max="11" width="31" style="3" customWidth="1"/>
-    <col min="12" max="12" width="30.44140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="32.33203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" style="3" customWidth="1"/>
-    <col min="16" max="18" width="24.109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="50.44140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="19.5546875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="19.21875" style="4" customWidth="1"/>
     <col min="19" max="19" width="48.88671875" style="3" customWidth="1"/>
-    <col min="20" max="22" width="29.6640625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="20.33203125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="20.21875" style="4" customWidth="1"/>
     <col min="23" max="23" width="30.6640625" style="3" customWidth="1"/>
     <col min="24" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:23" s="7" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
-    <row r="2" spans="1:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:23" s="7" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
     </row>
-    <row r="3" spans="1:23" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="7" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -590,7 +629,7 @@
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -645,8 +684,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="N5" s="5"/>
+    <row r="4" spans="1:23" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>